<commit_message>
Fertigstellung der zu druckenden Platine V2.1 und hinzufügen der Arbeitsplatzaustattung für das Löten
</commit_message>
<xml_diff>
--- a/doc/Stueckliste.xlsx
+++ b/doc/Stueckliste.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U0127601\Git\vierGewinnt\praktikum-4Gewinnt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2FC545E-EE4A-4822-8FDC-6D48644B1268}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA0B68D-8AA8-4944-A7A8-1F8E79AAB88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9B0BC8C6-C706-4EED-A247-6D2EB3940E10}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B0BC8C6-C706-4EED-A247-6D2EB3940E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -508,7 +508,7 @@
   <dimension ref="A1:C18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -691,8 +691,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Anleitung und Stücklisten angepasst
</commit_message>
<xml_diff>
--- a/doc/Stueckliste.xlsx
+++ b/doc/Stueckliste.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U0127601\Git\vierGewinnt\praktikum-4Gewinnt\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\U0127626\Git\Praktikum\neu\praktikum-4Gewinnt\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CA0B68D-8AA8-4944-A7A8-1F8E79AAB88B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{878A2665-F391-49E3-B436-D2C5BD4621F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{9B0BC8C6-C706-4EED-A247-6D2EB3940E10}"/>
+    <workbookView xWindow="11424" yWindow="0" windowWidth="11712" windowHeight="12336" xr2:uid="{9B0BC8C6-C706-4EED-A247-6D2EB3940E10}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>Stückliste</t>
   </si>
@@ -53,9 +53,6 @@
     <t>ESP32</t>
   </si>
   <si>
-    <t>5er 221-WAGO-Klemmen (6mm2)</t>
-  </si>
-  <si>
     <t>9V Batterie</t>
   </si>
   <si>
@@ -80,24 +77,15 @@
     <t>Spannungsregler (L7805ACV)</t>
   </si>
   <si>
-    <t>Diode (1N4007)</t>
-  </si>
-  <si>
     <t>Keramikkondensator (330 nF)</t>
   </si>
   <si>
     <t>Keramikkondensator (100 nF)</t>
   </si>
   <si>
-    <t>Elektrolytkondensator (1 µF)</t>
-  </si>
-  <si>
     <t>Bezeichnung</t>
   </si>
   <si>
-    <t>Vier_Gewinnt V1.0</t>
-  </si>
-  <si>
     <t>U2</t>
   </si>
   <si>
@@ -119,16 +107,13 @@
     <t>U1</t>
   </si>
   <si>
-    <t>D1</t>
-  </si>
-  <si>
     <t>C1</t>
   </si>
   <si>
     <t>C2</t>
   </si>
   <si>
-    <t>C3</t>
+    <t>Vier_Gewinnt V2.1</t>
   </si>
 </sst>
 </file>
@@ -197,8 +182,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6308B71C-8BED-44AB-8674-77AEB76E035C}" name="Tabelle1" displayName="Tabelle1" ref="A3:C18" totalsRowShown="0">
-  <autoFilter ref="A3:C18" xr:uid="{6308B71C-8BED-44AB-8674-77AEB76E035C}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{6308B71C-8BED-44AB-8674-77AEB76E035C}" name="Tabelle1" displayName="Tabelle1" ref="A3:C15" totalsRowShown="0">
+  <autoFilter ref="A3:C15" xr:uid="{6308B71C-8BED-44AB-8674-77AEB76E035C}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{191E4E9D-A626-4E13-A5C9-A16A04498F66}" name="Bauteil"/>
     <tableColumn id="2" xr3:uid="{C00D3819-A055-400E-804B-B9D440CB00BA}" name="Menge" dataDxfId="0"/>
@@ -505,10 +490,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A04CDECC-2BD7-4186-89EC-7796D3908BDB}">
-  <dimension ref="A1:C18"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="A3" sqref="A3:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -530,7 +515,7 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -541,7 +526,7 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -552,7 +537,7 @@
         <v>1</v>
       </c>
       <c r="C5" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -560,7 +545,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -568,7 +553,10 @@
         <v>6</v>
       </c>
       <c r="B7" s="2">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -576,10 +564,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="2">
-        <v>4</v>
-      </c>
-      <c r="C8" t="s">
-        <v>21</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -587,7 +572,10 @@
         <v>8</v>
       </c>
       <c r="B9" s="2">
-        <v>2</v>
+        <v>1</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -595,10 +583,10 @@
         <v>9</v>
       </c>
       <c r="B10" s="2">
-        <v>1</v>
+        <v>30</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -606,10 +594,10 @@
         <v>10</v>
       </c>
       <c r="B11" s="2">
-        <v>30</v>
+        <v>4</v>
       </c>
       <c r="C11" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -617,10 +605,10 @@
         <v>11</v>
       </c>
       <c r="B12" s="2">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="C12" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -631,7 +619,7 @@
         <v>1</v>
       </c>
       <c r="C13" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -642,7 +630,7 @@
         <v>1</v>
       </c>
       <c r="C14" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -653,40 +641,7 @@
         <v>1</v>
       </c>
       <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" s="2">
-        <v>1</v>
-      </c>
-      <c r="C16" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B17" s="2">
-        <v>1</v>
-      </c>
-      <c r="C17" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>17</v>
-      </c>
-      <c r="B18" s="2">
-        <v>1</v>
-      </c>
-      <c r="C18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>